<commit_message>
Adding system composition to SG supply database
The composition of primary, secondary and tertiary components constituting the supply system of specific predefined systems had not yet been updated for 'cooling' in the SG database. This has now been corrected.
</commit_message>
<xml_diff>
--- a/cea/databases/SG/assemblies/SUPPLY.xlsx
+++ b/cea/databases/SG/assemblies/SUPPLY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zshi/Documents/GitHub/CityEnergyAnalyst/cea/databases/SG/assemblies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Documents\GitHub\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\assemblies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6404D41B-F274-A24B-BF17-BC35734EAF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD659607-CF97-44B1-8DCC-5E322F264162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="31240" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEATING" sheetId="23" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
@@ -219,6 +219,24 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>CH1</t>
+  </si>
+  <si>
+    <t>CH2</t>
+  </si>
+  <si>
+    <t>CT2</t>
+  </si>
+  <si>
+    <t>CT1</t>
+  </si>
+  <si>
+    <t>AC1</t>
+  </si>
+  <si>
+    <t>HEX1</t>
   </si>
 </sst>
 </file>
@@ -226,9 +244,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -347,7 +365,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
@@ -360,16 +378,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -393,22 +411,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -417,7 +435,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,21 +721,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -809,20 +827,20 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,7 +872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -886,7 +904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -926,269 +944,333 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="12" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="65.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="11" max="11" width="43.83203125" customWidth="1"/>
+    <col min="1" max="1" width="65.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="21" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
+    <col min="14" max="14" width="43.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="15">
+      <c r="C2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="15">
         <v>0</v>
       </c>
-      <c r="G2" s="16">
+      <c r="J2" s="16">
         <v>0</v>
       </c>
-      <c r="H2" s="15">
+      <c r="K2" s="15">
         <v>20</v>
       </c>
-      <c r="I2" s="15">
+      <c r="L2" s="15">
         <v>1</v>
       </c>
-      <c r="J2" s="15">
-        <v>3</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="M2" s="15">
+        <v>3</v>
+      </c>
+      <c r="N2" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="H3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="18">
+      <c r="I3" s="18">
         <f>3.5168525/1.2808</f>
         <v>2.7458248750780765</v>
       </c>
-      <c r="G3" s="19">
-        <f>G4-63-79</f>
+      <c r="J3" s="19">
+        <f>J4-63-79</f>
         <v>710</v>
       </c>
-      <c r="H3" s="17">
+      <c r="K3" s="17">
         <v>20</v>
       </c>
-      <c r="I3" s="17">
-        <v>3</v>
-      </c>
-      <c r="J3" s="15">
-        <v>3</v>
-      </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="17">
+        <v>3</v>
+      </c>
+      <c r="M3" s="15">
+        <v>3</v>
+      </c>
+      <c r="N3" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="17">
+      <c r="I4" s="17">
         <v>3.88</v>
       </c>
-      <c r="G4" s="15">
+      <c r="J4" s="15">
         <v>852</v>
       </c>
-      <c r="H4" s="17">
+      <c r="K4" s="17">
         <v>20</v>
       </c>
-      <c r="I4" s="17">
+      <c r="L4" s="17">
         <v>4</v>
       </c>
-      <c r="J4" s="15">
-        <v>3</v>
-      </c>
-      <c r="K4" s="14" t="s">
+      <c r="M4" s="15">
+        <v>3</v>
+      </c>
+      <c r="N4" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="G5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="15">
+      <c r="I5" s="15">
         <v>6.5</v>
       </c>
-      <c r="G5" s="20">
-        <f>G6+430</f>
+      <c r="J5" s="20">
+        <f>J6+430</f>
         <v>1944</v>
       </c>
-      <c r="H5" s="17">
+      <c r="K5" s="17">
         <v>50</v>
       </c>
-      <c r="I5" s="17">
+      <c r="L5" s="17">
         <v>2.5</v>
       </c>
-      <c r="J5" s="15">
-        <v>3</v>
-      </c>
-      <c r="K5" s="14" t="s">
+      <c r="M5" s="15">
+        <v>3</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="9" customFormat="1" ht="78" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="G6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="H6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="23">
+      <c r="I6" s="23">
         <v>4.6399999999999997</v>
       </c>
-      <c r="G6" s="15">
+      <c r="J6" s="15">
         <v>1514</v>
       </c>
-      <c r="H6" s="23">
+      <c r="K6" s="23">
         <v>50</v>
       </c>
-      <c r="I6" s="23">
+      <c r="L6" s="23">
         <v>2</v>
       </c>
-      <c r="J6" s="15">
-        <v>3</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="M6" s="15">
+        <v>3</v>
+      </c>
+      <c r="N6" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="150" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="156" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="G7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="17">
+      <c r="I7" s="17">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G7" s="19">
+      <c r="J7" s="19">
         <v>271</v>
       </c>
-      <c r="H7" s="17">
+      <c r="K7" s="17">
         <v>15</v>
       </c>
-      <c r="I7" s="17">
+      <c r="L7" s="17">
         <v>12</v>
       </c>
-      <c r="J7" s="15">
-        <v>3</v>
-      </c>
-      <c r="K7" s="10" t="s">
+      <c r="M7" s="15">
+        <v>3</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1202,21 +1284,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1280,7 +1362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>

</xml_diff>